<commit_message>
modify the OCPTIME_ASSEMBLE_MAT_FOR_LS to OCPTIME_CONVERT_MAT_FOR_LS_IF
</commit_message>
<xml_diff>
--- a/data/scalingTest/refineComp/size.xlsx
+++ b/data/scalingTest/refineComp/size.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21094" windowHeight="8554"/>
+    <workbookView windowWidth="21094" windowHeight="9925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -705,7 +705,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -716,9 +716,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1038,7 +1035,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
@@ -1074,19 +1071,19 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1098,13 +1095,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="3">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="C2" s="3">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="D2" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1">
         <v>8325</v>
@@ -1123,19 +1120,19 @@
         <v>10000</v>
       </c>
       <c r="L2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2" s="4">
         <v>10000</v>
       </c>
       <c r="N2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O2" s="4">
         <v>100</v>
       </c>
       <c r="P2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1149,19 +1146,19 @@
         <v>5000</v>
       </c>
       <c r="L3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M3" s="4">
         <v>5000</v>
       </c>
       <c r="N3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O3" s="4">
         <v>50</v>
       </c>
       <c r="P3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1175,19 +1172,19 @@
         <v>2500</v>
       </c>
       <c r="L4" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M4" s="4">
         <v>2500</v>
       </c>
       <c r="N4" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="O4" s="4">
         <v>25</v>
       </c>
       <c r="P4" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1201,19 +1198,19 @@
         <v>1250</v>
       </c>
       <c r="L5" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="M5" s="4">
         <v>1250</v>
       </c>
       <c r="N5" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="O5" s="4">
         <v>12</v>
       </c>
       <c r="P5" s="1">
-        <v>25</v>
+        <v>8.3</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1230,19 +1227,19 @@
         <v>625</v>
       </c>
       <c r="L6" s="1">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="M6" s="4">
         <v>625</v>
       </c>
       <c r="N6" s="1">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="O6" s="4">
         <v>6</v>
       </c>
       <c r="P6" s="1">
-        <v>50</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="7" spans="1:16">

</xml_diff>

<commit_message>
change size of test case
</commit_message>
<xml_diff>
--- a/data/scalingTest/refineComp/size.xlsx
+++ b/data/scalingTest/refineComp/size.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21094" windowHeight="9925"/>
+    <workbookView windowWidth="21094" windowHeight="8554"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>UNIT</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>512n</t>
+  </si>
+  <si>
+    <t>64n</t>
+  </si>
+  <si>
+    <t>8n</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>7p</t>
   </si>
   <si>
     <t>PermX</t>
@@ -705,7 +720,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,6 +734,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1035,14 +1053,14 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
   <cols>
     <col min="1" max="1" width="11.5765765765766" customWidth="1"/>
     <col min="2" max="6" width="9.46846846846847"/>
-    <col min="10" max="10" width="9.46846846846847"/>
+    <col min="10" max="10" width="13.1261261261261" customWidth="1"/>
     <col min="16" max="16" width="20.6036036036036" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1095,13 +1113,16 @@
         <v>14</v>
       </c>
       <c r="B2" s="3">
-        <v>10000</v>
+        <f>K2*L2</f>
+        <v>16000</v>
       </c>
       <c r="C2" s="3">
-        <v>10000</v>
+        <f>M2*N2</f>
+        <v>16000</v>
       </c>
       <c r="D2" s="3">
-        <v>100</v>
+        <f>O2*P2</f>
+        <v>200</v>
       </c>
       <c r="E2" s="1">
         <v>8325</v>
@@ -1112,105 +1133,117 @@
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="J2" s="2">
         <f>K2*M2*O2</f>
-        <v>10000000000</v>
+        <v>1024000000</v>
       </c>
       <c r="K2" s="4">
-        <v>10000</v>
+        <v>1600</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M2" s="4">
-        <v>10000</v>
+        <v>1600</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O2" s="4">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="P2" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1"/>
       <c r="E3" s="2"/>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="J3" s="2">
         <f>K3*M3*O3</f>
-        <v>1250000000</v>
+        <v>128000000</v>
       </c>
       <c r="K3" s="4">
-        <v>5000</v>
+        <v>800</v>
       </c>
       <c r="L3" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M3" s="4">
-        <v>5000</v>
+        <v>800</v>
       </c>
       <c r="N3" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="O3" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="P3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1"/>
       <c r="E4" s="1"/>
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J4" s="2">
         <f>K4*M4*O4</f>
-        <v>156250000</v>
+        <v>16000000</v>
       </c>
       <c r="K4" s="4">
-        <v>2500</v>
+        <v>400</v>
       </c>
       <c r="L4" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="M4" s="4">
-        <v>2500</v>
+        <v>400</v>
       </c>
       <c r="N4" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="O4" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="P4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="E5" s="1"/>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="J5" s="2">
         <f>K5*M5*O5</f>
-        <v>18750000</v>
+        <v>2000000</v>
       </c>
       <c r="K5" s="4">
-        <v>1250</v>
+        <v>200</v>
       </c>
       <c r="L5" s="1">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="M5" s="4">
-        <v>1250</v>
+        <v>200</v>
       </c>
       <c r="N5" s="1">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="O5" s="4">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="P5" s="1">
-        <v>8.3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1219,39 +1252,42 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="J6" s="2">
         <f>K6*M6*O6</f>
-        <v>2343750</v>
+        <v>250000</v>
       </c>
       <c r="K6" s="4">
-        <v>625</v>
+        <v>100</v>
       </c>
       <c r="L6" s="1">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="M6" s="4">
-        <v>625</v>
+        <v>100</v>
       </c>
       <c r="N6" s="1">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="O6" s="4">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="P6" s="1">
-        <v>16.7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
@@ -1268,7 +1304,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1">
         <v>500</v>
@@ -1290,7 +1326,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
         <v>50</v>
@@ -1312,7 +1348,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>200</v>

</xml_diff>